<commit_message>
Changes on Names For Paper
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/Temporary_ToHelpBuildDecks/TMP_ExistingCapacity_UniqueTechNameLv2.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/Temporary_ToHelpBuildDecks/TMP_ExistingCapacity_UniqueTechNameLv2.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DFO_IC_Existing</t>
+          <t>DFO_IC_EXISTING</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NUC_ST_Existing</t>
+          <t>NUC_ST_EXISTING</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NG_GT_Existing</t>
+          <t>NG_GT_EXISTING</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NG_CC_Existing</t>
+          <t>NG_CC_EXISTING</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLQ_ST_Existing</t>
+          <t>BLQ_ST_EXISTING</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SUN_PV_Existing</t>
+          <t>SUN_PV_EXISTING</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MWH_BA1h_Existing</t>
+          <t>MWH_BA1H_EXISTING</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DFO_GT_Existing</t>
+          <t>DFO_GT_EXISTING</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>WDS_ST_Existing</t>
+          <t>WDS_ST_EXISTING</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>WH_ST_Existing</t>
+          <t>WH_ST_EXISTING</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LFG_IC_Existing</t>
+          <t>LFG_IC_EXISTING</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>WND_WT_Existing</t>
+          <t>WND_WT_EXISTING</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AB_ST_Existing</t>
+          <t>AB_ST_EXISTING</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>NG_ST_Existing</t>
+          <t>NG_ST_EXISTING</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>WAT_HY_Existing</t>
+          <t>WAT_HY_EXISTING</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WAT_PS_Existing</t>
+          <t>WAT_PS_EXISTING</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DFO_CC_Existing</t>
+          <t>DFO_CC_EXISTING</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BIT_ST_Existing</t>
+          <t>BIT_ST_EXISTING</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LFG_GT_Existing</t>
+          <t>LFG_GT_EXISTING</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>OBG_IC_Existing</t>
+          <t>OBG_IC_EXISTING</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MWH_BA2h_Existing</t>
+          <t>MWH_BA2H_EXISTING</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">

</xml_diff>